<commit_message>
Add scraping halman with infinite scroll
</commit_message>
<xml_diff>
--- a/Properties.xlsx
+++ b/Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giorg\Documents\Projects\UpworkRepos\real-estate-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B238AB-5E3D-4CE4-8C99-3A3CAEE5503D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30BFA73-2E81-4AAA-A007-5C642DBF9534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rightmove" sheetId="1" r:id="rId1"/>
@@ -364,8 +364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,7 +381,8 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
   </sheetData>
@@ -392,10 +393,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,6 +421,9 @@
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -427,19 +431,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A25" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="103.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Infinite scroll on halman
</commit_message>
<xml_diff>
--- a/Properties.xlsx
+++ b/Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giorg\Documents\Projects\UpworkRepos\real-estate-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30BFA73-2E81-4AAA-A007-5C642DBF9534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD97A17C-DD72-4F0A-85D4-DC8E05089D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rightmove" sheetId="1" r:id="rId1"/>
@@ -364,13 +364,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A2:A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="100.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A2:A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>